<commit_message>
Added code to incorporate for missing data from events
</commit_message>
<xml_diff>
--- a/DateNamePairings.xlsx
+++ b/DateNamePairings.xlsx
@@ -1,42 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rowanscassellati/Documents/GitHub/WCC_Deishacks_Visualizations/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62CDB9F5-9940-7E43-837B-408D9E92C521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="13820" xr2:uid="{8A937158-8853-504B-8C95-074468A1B6C1}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -60,25 +38,44 @@
   </si>
   <si>
     <t>Oh I Had An Idea</t>
+  </si>
+  <si>
+    <t>Here is a New Name!</t>
+  </si>
+  <si>
+    <t>This is also a new one!</t>
+  </si>
+  <si>
+    <t>Created on Saturday</t>
+  </si>
+  <si>
+    <t>This is in December</t>
+  </si>
+  <si>
+    <t>AAAAAAA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -90,12 +87,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -104,22 +116,16 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -134,44 +140,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -198,32 +204,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -250,24 +238,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -279,176 +249,178 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr"/>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD729F0-1DBE-6349-97A4-054BBD7F17AE}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>44215</v>
       </c>
@@ -476,7 +448,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>44742</v>
       </c>
@@ -490,7 +462,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>44806</v>
       </c>
@@ -504,7 +476,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2">
         <v>44195</v>
       </c>
@@ -516,6 +488,91 @@
       </c>
       <c r="D5">
         <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2">
+        <v>44253</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2">
+        <v>44143</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2">
+        <v>44316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>45</v>
+      </c>
+      <c r="D9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2">
+        <v>44189</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2">
+        <v>44169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2">
+        <v>44823</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>40</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2">
+        <v>44606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Information for Specific Events
</commit_message>
<xml_diff>
--- a/DateNamePairings.xlsx
+++ b/DateNamePairings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -46,13 +46,10 @@
     <t>This is also a new one!</t>
   </si>
   <si>
-    <t>Created on Saturday</t>
-  </si>
-  <si>
-    <t>This is in December</t>
-  </si>
-  <si>
-    <t>AAAAAAA</t>
+    <t>Saturday Night</t>
+  </si>
+  <si>
+    <t>Another Saturday Night</t>
   </si>
 </sst>
 </file>
@@ -525,54 +522,45 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>44072</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>45</v>
-      </c>
-      <c r="D9">
-        <v>23</v>
+        <v>44823</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>44189</v>
+        <v>44606</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
+        <v>35</v>
+      </c>
+      <c r="D10">
         <v>50</v>
-      </c>
-      <c r="D10">
-        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
         <v>44169</v>
       </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>75</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>44823</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>40</v>
-      </c>
-      <c r="D12">
-        <v>50</v>
+        <v>44189</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>44606</v>
+        <v>44072</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed out of bounds errors
</commit_message>
<xml_diff>
--- a/DateNamePairings.xlsx
+++ b/DateNamePairings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Another Saturday Night</t>
+  </si>
+  <si>
+    <t>Event Name Here90</t>
   </si>
 </sst>
 </file>
@@ -411,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -563,6 +566,20 @@
         <v>44072</v>
       </c>
     </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2">
+        <v>45682</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>89</v>
+      </c>
+      <c r="D14">
+        <v>899</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated date-name pairings for example code
</commit_message>
<xml_diff>
--- a/DateNamePairings.xlsx
+++ b/DateNamePairings.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rowanscassellati/Documents/GitHub/WCC_Deishacks_Visualizations/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA23A1D-4652-164E-B389-AB6A4C9B2FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="24180" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -28,41 +47,191 @@
     <t>Price for Members</t>
   </si>
   <si>
-    <t>What?</t>
-  </si>
-  <si>
-    <t>Madeline</t>
-  </si>
-  <si>
-    <t>Caitlyn</t>
-  </si>
-  <si>
-    <t>Oh I Had An Idea</t>
-  </si>
-  <si>
-    <t>Here is a New Name!</t>
-  </si>
-  <si>
-    <t>This is also a new one!</t>
-  </si>
-  <si>
-    <t>Saturday Night</t>
-  </si>
-  <si>
-    <t>Another Saturday Night</t>
-  </si>
-  <si>
-    <t>Event Name Here90</t>
+    <t>2020-09-05</t>
+  </si>
+  <si>
+    <t>2023-06-11</t>
+  </si>
+  <si>
+    <t>2021-09-15</t>
+  </si>
+  <si>
+    <t>2022-05-09</t>
+  </si>
+  <si>
+    <t>2020-09-22</t>
+  </si>
+  <si>
+    <t>2024-01-26</t>
+  </si>
+  <si>
+    <t>2020-03-27</t>
+  </si>
+  <si>
+    <t>2021-11-17</t>
+  </si>
+  <si>
+    <t>2020-06-10</t>
+  </si>
+  <si>
+    <t>2023-08-07</t>
+  </si>
+  <si>
+    <t>2021-04-06</t>
+  </si>
+  <si>
+    <t>2021-12-02</t>
+  </si>
+  <si>
+    <t>2023-09-03</t>
+  </si>
+  <si>
+    <t>2023-08-19</t>
+  </si>
+  <si>
+    <t>2020-11-07</t>
+  </si>
+  <si>
+    <t>2024-07-31</t>
+  </si>
+  <si>
+    <t>2022-08-26</t>
+  </si>
+  <si>
+    <t>2023-01-23</t>
+  </si>
+  <si>
+    <t>2023-07-12</t>
+  </si>
+  <si>
+    <t>2023-12-20</t>
+  </si>
+  <si>
+    <t>2022-11-28</t>
+  </si>
+  <si>
+    <t>2022-09-26</t>
+  </si>
+  <si>
+    <t>2020-09-21</t>
+  </si>
+  <si>
+    <t>2024-05-24</t>
+  </si>
+  <si>
+    <t>2024-05-22</t>
+  </si>
+  <si>
+    <t>2020-11-05</t>
+  </si>
+  <si>
+    <t>2023-03-23</t>
+  </si>
+  <si>
+    <t>2021-03-13</t>
+  </si>
+  <si>
+    <t>2023-12-21</t>
+  </si>
+  <si>
+    <t>2020-04-20</t>
+  </si>
+  <si>
+    <t>Waltham Business Expo</t>
+  </si>
+  <si>
+    <t>Innovate Waltham: Business Leaders Summit</t>
+  </si>
+  <si>
+    <t>Waltham Women in Business Roundtable</t>
+  </si>
+  <si>
+    <t>Chamber Connect: Networking Breakfast</t>
+  </si>
+  <si>
+    <t>Tech Talks: Waltham’s Future in Innovation</t>
+  </si>
+  <si>
+    <t>Leadership Lunch &amp; Learn</t>
+  </si>
+  <si>
+    <t>Economic Insights: Waltham’s Growth Forecast</t>
+  </si>
+  <si>
+    <t>After Hours Business Mixer</t>
+  </si>
+  <si>
+    <t>Small Business Success Workshop</t>
+  </si>
+  <si>
+    <t>Waltham Business Awards Gala</t>
+  </si>
+  <si>
+    <t>Startup Showcase: Waltham’s Emerging Ventures</t>
+  </si>
+  <si>
+    <t>Green Business Forum: Sustainability in Waltham</t>
+  </si>
+  <si>
+    <t>Business Speed Networking Night</t>
+  </si>
+  <si>
+    <t>Community Commerce Fair</t>
+  </si>
+  <si>
+    <t>Waltham Business &amp; Beer Social</t>
+  </si>
+  <si>
+    <t>Chamber Charity Golf Tournament</t>
+  </si>
+  <si>
+    <t>Diversity in Business: A Waltham Perspective</t>
+  </si>
+  <si>
+    <t>Future of Work: Workforce Development in Waltham</t>
+  </si>
+  <si>
+    <t>Chamber Coffee Chat: Meet the Board</t>
+  </si>
+  <si>
+    <t>Annual Business Appreciation Luncheon</t>
+  </si>
+  <si>
+    <t>Chamber Leadership Retreat</t>
+  </si>
+  <si>
+    <t>Waltham Entrepreneurs' Bootcamp</t>
+  </si>
+  <si>
+    <t>Business Innovation Pitch Night</t>
+  </si>
+  <si>
+    <t>Professional Development Power Hour</t>
+  </si>
+  <si>
+    <t>Local Business Marketplace Expo</t>
+  </si>
+  <si>
+    <t>Business Resilience and Recovery Forum</t>
+  </si>
+  <si>
+    <t>Future Leaders Networking Night</t>
+  </si>
+  <si>
+    <t>Tech &amp; Trends: Insights for Tomorrow</t>
+  </si>
+  <si>
+    <t>Chamber Holiday Business Gala</t>
+  </si>
+  <si>
+    <t>Building Bridges: Community &amp; Commerce Summit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,20 +288,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -170,7 +347,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -204,6 +381,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -238,9 +416,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -413,14 +592,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,150 +615,424 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2">
-        <v>44215</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2">
-        <v>44742</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3">
         <v>40</v>
       </c>
-      <c r="D3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
         <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2">
-        <v>44806</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>40</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2">
-        <v>44195</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6">
+        <v>65</v>
+      </c>
+      <c r="D6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7">
         <v>50</v>
       </c>
-      <c r="D5">
+      <c r="D7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2">
-        <v>44253</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
+      <c r="C8">
+        <v>65</v>
+      </c>
+      <c r="D8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9">
         <v>40</v>
       </c>
-      <c r="D6">
+      <c r="D9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10">
+        <v>75</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11">
+        <v>55</v>
+      </c>
+      <c r="D11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12">
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13">
+        <v>55</v>
+      </c>
+      <c r="D13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
+        <v>55</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15">
+        <v>55</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16">
+        <v>55</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>55</v>
+      </c>
+      <c r="D18">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20">
+        <v>55</v>
+      </c>
+      <c r="D20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22">
+        <v>75</v>
+      </c>
+      <c r="D22">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23">
+        <v>55</v>
+      </c>
+      <c r="D23">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24">
+        <v>40</v>
+      </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25">
+        <v>40</v>
+      </c>
+      <c r="D25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26">
+        <v>55</v>
+      </c>
+      <c r="D26">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2">
-        <v>44143</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
+      <c r="D27">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2">
-        <v>44316</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2">
-        <v>44823</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2">
-        <v>44606</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28">
+        <v>40</v>
+      </c>
+      <c r="D28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29">
+        <v>70</v>
+      </c>
+      <c r="D29">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30">
+        <v>25</v>
+      </c>
+      <c r="D30">
         <v>10</v>
       </c>
-      <c r="C10">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31">
         <v>35</v>
       </c>
-      <c r="D10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2">
-        <v>44169</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <v>75</v>
-      </c>
-      <c r="D11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2">
-        <v>44189</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="2">
-        <v>44072</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2">
-        <v>45682</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>89</v>
-      </c>
-      <c r="D14">
-        <v>899</v>
+      <c r="D31">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>